<commit_message>
Improved documentation and test data
</commit_message>
<xml_diff>
--- a/resource/example/user-story-denormalized-data.xlsx
+++ b/resource/example/user-story-denormalized-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Solution Developer</t>
   </si>
   <si>
     <t>Business Analyst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quickly and easily test my code in my test Cloud environment that is deployed in a similar way to the production environment </t>
   </si>
   <si>
     <t>deploy the Repository in my test Cloud</t>
@@ -71,6 +68,21 @@
   </si>
   <si>
     <t>try out writing some apps using it</t>
+  </si>
+  <si>
+    <t>Beatle</t>
+  </si>
+  <si>
+    <t>hold your hand</t>
+  </si>
+  <si>
+    <t>The song must be less than three minutes long</t>
+  </si>
+  <si>
+    <t>have a hit single</t>
+  </si>
+  <si>
+    <t>quickly and easily test my code in my test Cloud environment</t>
   </si>
 </sst>
 </file>
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -659,88 +671,88 @@
     <col min="4" max="4" width="58" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45">
-      <c r="A1" s="4" t="s">
-        <v>5</v>
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="66">
@@ -748,41 +760,55 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="66">
+      <c r="A8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45">
       <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
+    </row>
+    <row r="10" spans="1:4" ht="45">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>